<commit_message>
Fit the logistic curve for the pre-season forecast
</commit_message>
<xml_diff>
--- a/pre-season-forecast/fit_logistic.xlsx
+++ b/pre-season-forecast/fit_logistic.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryce/src/2019-yukon-forecasting/may_forecast/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\src\yukon-forecasting\2022-forecast\pre-season-forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4D8EBF-A9E2-4947-9B17-A1D9EB05154D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="3040" windowWidth="26300" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="3038" windowWidth="26303" windowHeight="15383" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +19,7 @@
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
@@ -29,6 +29,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$5</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
@@ -41,12 +42,12 @@
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>r</t>
   </si>
@@ -77,19 +78,13 @@
   </si>
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>frombelow</t>
-  </si>
-  <si>
-    <t>fromabove</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -431,16 +426,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -457,48 +452,48 @@
         <v>5</v>
       </c>
       <c r="G1">
-        <v>18.055015287043943</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>18.007274784929372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>0.15</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>1/(1+EXP(-((B2-$G$1)/$G$2)))</f>
-        <v>0.14022098104808176</v>
+        <v>0.14869508185945346</v>
       </c>
       <c r="D2">
         <f>C2-A2</f>
-        <v>-9.7790189519182391E-3</v>
+        <v>-1.3049181405465349E-3</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2">
-        <v>3.890370714602347</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>4.5890312131293562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>0.25</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C4" si="0">1/(1+EXP(-((B3-$G$1)/$G$2)))</f>
-        <v>0.26070239414905783</v>
+        <v>0.25140369980996868</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D4" si="1">C3-A3</f>
-        <v>1.0702394149057826E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>1.4036998099686837E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -507,57 +502,27 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>0.49646470900383827</v>
+        <v>0.49960368631918012</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>-3.5352909961617329E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-3.9631368081988194E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5">
         <f>SUMSQ(D2:D4)</f>
-        <v>2.2266873461130549E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="H9">
-        <v>18.05502460989219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="H10">
-        <v>3.8904097513825908</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13">
-        <v>18.055002113649405</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="H14">
-        <v>3.8903789442715091</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8">
-      <c r="G17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="1">
-        <v>18.055015300000001</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8">
-      <c r="H18" s="1">
-        <v>3.89037071</v>
-      </c>
+        <v>3.830249043638548E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>